<commit_message>
modificaciones en el envio de correos
</commit_message>
<xml_diff>
--- a/data/data_cus.xlsx
+++ b/data/data_cus.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t>cedula</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Fallido</t>
-  </si>
-  <si>
-    <t>28/01/2025 11:22 AM</t>
   </si>
   <si>
     <t>Pago de servicio de electricidad</t>
@@ -510,6 +507,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="36.88"/>
     <col customWidth="1" min="7" max="7" width="20.88"/>
   </cols>
   <sheetData>
@@ -538,7 +536,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -561,7 +559,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -584,7 +582,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
@@ -607,16 +605,16 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>1.112223334E9</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>1.010788877E9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.013292145E9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="2">
         <v>1.234509876E9</v>
@@ -630,16 +628,16 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E6" s="2">
         <v>5.43216789E9</v>
@@ -653,16 +651,16 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>6.789012345E9</v>
@@ -676,16 +674,16 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E8" s="2">
         <v>1.234098765E9</v>
@@ -699,16 +697,16 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E9" s="2">
         <v>4.321098765E9</v>
@@ -722,13 +720,13 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -745,16 +743,16 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>1.112223334E9</v>
+        <v>1.010788877E9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E11" s="2">
         <v>2.345678901E9</v>
@@ -768,16 +766,16 @@
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="2">
         <v>9.876543212E9</v>
@@ -791,16 +789,16 @@
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E13" s="2">
         <v>7.654321098E9</v>
@@ -814,13 +812,13 @@
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -837,16 +835,16 @@
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E15" s="2">
         <v>4.321098754E9</v>
@@ -860,13 +858,13 @@
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
@@ -883,16 +881,16 @@
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2">
         <v>9.876540987E9</v>
@@ -906,16 +904,16 @@
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2">
         <v>1.234567809E9</v>
@@ -929,16 +927,16 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2">
         <v>7.65432198E9</v>
@@ -952,16 +950,16 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="2">
         <v>1.234098761E9</v>
@@ -975,16 +973,16 @@
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>2.223334445E9</v>
+        <v>6.2455663E7</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="E21" s="2">
         <v>5.678904321E9</v>
@@ -998,16 +996,16 @@
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="2">
         <v>8.765432198E9</v>
@@ -1021,16 +1019,16 @@
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="E23" s="2">
         <v>9.876543213E9</v>
@@ -1044,16 +1042,16 @@
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E24" s="2">
         <v>1.234567893E9</v>
@@ -1067,16 +1065,16 @@
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2">
         <v>4.32109876E9</v>
@@ -1090,16 +1088,16 @@
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="2">
         <v>5.432178909E9</v>
@@ -1113,16 +1111,16 @@
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="E27" s="2">
         <v>6.789012456E9</v>
@@ -1136,13 +1134,13 @@
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>13</v>
@@ -1159,16 +1157,16 @@
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="2">
         <v>4.321098764E9</v>
@@ -1182,16 +1180,16 @@
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2">
         <v>1.234567894E9</v>
@@ -1205,16 +1203,16 @@
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>3.334445556E9</v>
+        <v>1.013292145E9</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="E31" s="2">
         <v>5.678901243E9</v>

</xml_diff>

<commit_message>
cambio de excel a csv por problemas de compatibilidad
</commit_message>
<xml_diff>
--- a/data/data_cus.xlsx
+++ b/data/data_cus.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>cedula</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Fallido</t>
+  </si>
+  <si>
+    <t>29/01/2025 08:40 PM</t>
   </si>
   <si>
     <t>Pago de servicio de electricidad</t>
@@ -607,14 +610,14 @@
       <c r="A5" s="2">
         <v>1.010788877E9</v>
       </c>
-      <c r="B5" s="2">
-        <v>1.013292145E9</v>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2">
         <v>1.234509876E9</v>
@@ -631,13 +634,13 @@
         <v>1.010788877E9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
         <v>5.43216789E9</v>
@@ -654,13 +657,13 @@
         <v>1.010788877E9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>6.789012345E9</v>
@@ -677,13 +680,13 @@
         <v>1.010788877E9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2">
         <v>1.234098765E9</v>
@@ -700,13 +703,13 @@
         <v>1.010788877E9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2">
         <v>4.321098765E9</v>
@@ -723,10 +726,10 @@
         <v>1.010788877E9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -746,13 +749,13 @@
         <v>1.010788877E9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2">
         <v>2.345678901E9</v>
@@ -769,13 +772,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2">
         <v>9.876543212E9</v>
@@ -792,13 +795,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2">
         <v>7.654321098E9</v>
@@ -815,10 +818,10 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -838,13 +841,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="2">
         <v>4.321098754E9</v>
@@ -861,10 +864,10 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
@@ -884,13 +887,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2">
         <v>9.876540987E9</v>
@@ -907,13 +910,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E18" s="2">
         <v>1.234567809E9</v>
@@ -930,13 +933,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="2">
         <v>7.65432198E9</v>
@@ -953,13 +956,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E20" s="2">
         <v>1.234098761E9</v>
@@ -976,13 +979,13 @@
         <v>6.2455663E7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" s="2">
         <v>5.678904321E9</v>
@@ -999,13 +1002,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2">
         <v>8.765432198E9</v>
@@ -1022,13 +1025,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E23" s="2">
         <v>9.876543213E9</v>
@@ -1045,13 +1048,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E24" s="2">
         <v>1.234567893E9</v>
@@ -1068,13 +1071,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="2">
         <v>4.32109876E9</v>
@@ -1091,13 +1094,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2">
         <v>5.432178909E9</v>
@@ -1114,13 +1117,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E27" s="2">
         <v>6.789012456E9</v>
@@ -1137,10 +1140,10 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>13</v>
@@ -1160,13 +1163,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E29" s="2">
         <v>4.321098764E9</v>
@@ -1183,13 +1186,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E30" s="2">
         <v>1.234567894E9</v>
@@ -1206,13 +1209,13 @@
         <v>1.013292145E9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="2">
         <v>5.678901243E9</v>

</xml_diff>